<commit_message>
add new funs to get data
</commit_message>
<xml_diff>
--- a/Optimizer_matlab/config/opt_project_config_daily.xlsx
+++ b/Optimizer_matlab/config/opt_project_config_daily.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\qlib-optimizer\Optimizer_matlab\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DB137F-5F40-4614-83EE-EBCE4A91B758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9400DA2-AE1A-4228-86C3-960EFA2F12FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="1935" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5475" yWindow="3615" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="导出摘要" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="130">
   <si>
     <t>此文稿由 Numbers 表格导出。所有表格均已转换为 Excel 工作表。每张 Numbers 工作表上的所有其他对象都已放置在单独的工作表中。请注意其中的公式计算可能与 Excel 不同。</t>
   </si>
@@ -347,17 +347,6 @@
   <si>
     <t>vp08</t>
     <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>中证500</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>中证500</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>中证A500</t>
   </si>
   <si>
     <t>fm01_hs300_HB</t>
@@ -722,7 +711,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -812,13 +801,7 @@
     <xf numFmtId="49" fontId="8" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2017,11 +2000,11 @@
     </row>
     <row r="3" spans="1:5" ht="50.1" customHeight="1">
       <c r="A3" s="8"/>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
       <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" ht="15.95" customHeight="1">
@@ -2170,10 +2153,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="A3" sqref="A3:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" customHeight="1"/>
@@ -2206,7 +2189,7 @@
     </row>
     <row r="2" spans="1:5" ht="15.95" customHeight="1">
       <c r="A2" s="20" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B2" s="32" t="s">
         <v>103</v>
@@ -2218,91 +2201,6 @@
         <v>14</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.95" customHeight="1">
-      <c r="A3" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.95" customHeight="1">
-      <c r="A4" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.95" customHeight="1">
-      <c r="A5" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A6" s="35" t="s">
-        <v>131</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="19" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2369,16 +2267,16 @@
         <v>21</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H1" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" s="22" t="s">
         <v>115</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>118</v>
       </c>
       <c r="K1" s="21" t="s">
         <v>22</v>
@@ -2393,16 +2291,16 @@
         <v>24</v>
       </c>
       <c r="O1" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q1" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="R1" s="21" t="s">
         <v>119</v>
-      </c>
-      <c r="P1" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q1" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="R1" s="21" t="s">
-        <v>122</v>
       </c>
       <c r="S1" s="21" t="s">
         <v>25</v>
@@ -2429,16 +2327,16 @@
         <v>32</v>
       </c>
       <c r="AA1" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB1" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC1" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="AD1" s="22" t="s">
         <v>123</v>
-      </c>
-      <c r="AB1" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="AC1" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="AD1" s="22" t="s">
-        <v>126</v>
       </c>
       <c r="AE1" s="22"/>
       <c r="AF1" s="22"/>
@@ -6239,47 +6137,47 @@
       <c r="A1" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="H1" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="E1" s="34" t="s">
+      <c r="K1" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="M1" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="N1" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="F1" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="H1" s="36" t="s">
+      <c r="O1" s="33" t="s">
         <v>129</v>
-      </c>
-      <c r="I1" s="36" t="s">
-        <v>130</v>
-      </c>
-      <c r="J1" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="K1" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="L1" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="M1" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="N1" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="O1" s="34" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.95" customHeight="1">

</xml_diff>